<commit_message>
Regenerated file to remove Google Sharing status in an attempt to repair repository
</commit_message>
<xml_diff>
--- a/UAZ_Refined.xlsx
+++ b/UAZ_Refined.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Collection Management\Research\Santa Catalinas Survey Results\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Collection Management\Research\Santa Catalinas Survey Results\Data\SC OccRecords Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E6D967-2295-4D75-A0B4-9636A9E0D980}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E1C321-7816-4A7D-808C-CE54DCC5C7DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>